<commit_message>
feat: expense search button added
</commit_message>
<xml_diff>
--- a/FinanceApp/Template/ImportExpenses.xlsx
+++ b/FinanceApp/Template/ImportExpenses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hpnol\source\repos\FinanceAppV2\FinanceApp\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD7FDB6E-6E5E-4142-8082-8E039CD7A531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B8E03B6-FFEE-4EAF-AE01-18122C878D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="5">
   <si>
     <t>Description</t>
   </si>
@@ -367,10 +367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A9" sqref="A9:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -401,6 +401,83 @@
       </c>
       <c r="F2" s="1"/>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2000</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2000</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2000</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2000</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2000</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2000</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2000</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>